<commit_message>
Add stage 3 (B1-B2)
</commit_message>
<xml_diff>
--- a/szryldrm/evidence.xlsx
+++ b/szryldrm/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\1W_szryldrm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_szryldrm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F84EE6-6914-40C1-9FF1-219AE7097E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39EC33B-ED82-45BF-ADB0-107512C6FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
   <si>
     <t>TxHash</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>5421945DF6D69EBFAD44086093FED32020C9F10E1C65A6A6705327847F33339B</t>
+  </si>
+  <si>
+    <t>C16D20B44314B3FBEAC198EDDA69A738937AE90AE5F4E0BD64104F321BF82FB3</t>
+  </si>
+  <si>
+    <t>AAADE957FDF44AEF092AC887F3ACAB1EA1E12CFC11E9E9EC483282055FA116CB</t>
+  </si>
+  <si>
+    <t>8D377032E6CBEFC276C68FF3AA35C1126474E26D31CABFDE138BB2FF46D32271</t>
+  </si>
+  <si>
+    <t>85E290743B46237632CD731B55E4987732757AA29A8415FE3D610CAF4E92ED0C</t>
   </si>
 </sst>
 </file>
@@ -237,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -251,6 +263,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -560,7 +575,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1203,7 +1218,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1217,12 +1234,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1254,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1251,12 +1270,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Round 4 evidences (B5/B6/B7)
</commit_message>
<xml_diff>
--- a/szryldrm/evidence.xlsx
+++ b/szryldrm/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_szryldrm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39EC33B-ED82-45BF-ADB0-107512C6FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F97847-4609-4D27-B9A1-8329048EBD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" firstSheet="2" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" firstSheet="5" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -176,6 +171,24 @@
   </si>
   <si>
     <t>85E290743B46237632CD731B55E4987732757AA29A8415FE3D610CAF4E92ED0C</t>
+  </si>
+  <si>
+    <t>167D5497C8BE5959EAD8FBE6E6A161DE0AB3F5876D75E4842D7687608C8F5498</t>
+  </si>
+  <si>
+    <t>6B80D59FACF3D00506EB0C527A327918AA037D97FEB83BC4551CA3F1BC5BFCCB</t>
+  </si>
+  <si>
+    <t>9396A978EA035444E7BEBBFED39C0362A2104660218B65B28D9EE926D9F56899</t>
+  </si>
+  <si>
+    <t>134ED7CE15C61C56E4A88E723B0E49140B7FC7BB8A3186EF922E89D5E1C0EB33</t>
+  </si>
+  <si>
+    <t>7CBEEAB11F2AB1AE8A98D03C0D2C28055FD3C49A3995FACA4919EF7FD3B65E73</t>
+  </si>
+  <si>
+    <t>388C83D2189F82AA31DE36A73197E4091CC88DBB44C873B0EBFA67D055342D38</t>
   </si>
 </sst>
 </file>
@@ -593,51 +606,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -663,18 +676,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -699,18 +712,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -735,18 +748,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -771,18 +784,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -810,26 +823,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -858,26 +871,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -906,26 +919,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -954,26 +967,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -1002,26 +1015,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -1050,26 +1063,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -1099,15 +1112,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1135,26 +1148,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -1183,26 +1196,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
@@ -1234,12 +1247,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1254,7 +1267,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1270,12 +1283,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1303,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1304,12 +1319,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1324,7 +1339,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1338,12 +1355,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE35878B-2203-4669-B881-5C4129774FBE}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1373,32 +1423,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1430,27 +1480,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1481,27 +1531,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1532,27 +1582,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1584,27 +1634,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1629,18 +1679,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1665,20 +1715,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add evidences for A7 to A20
</commit_message>
<xml_diff>
--- a/szryldrm/evidence.xlsx
+++ b/szryldrm/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_0k_szryldrm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\_A1-A20 eksik_szryldrm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F97847-4609-4D27-B9A1-8329048EBD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D274FD-9654-4C58-8368-9D2DA74F6604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" firstSheet="5" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>TxHash</t>
   </si>
@@ -53,27 +53,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -119,48 +104,12 @@
     <t>uptick1tn3xyys4w8slmrfvfjqy97gydjp3v349g7u6ap</t>
   </si>
   <si>
-    <t>DB83E98DDCF3245CB862BDF9268887E446D913DCA7E370962741E8697EC410CE</t>
-  </si>
-  <si>
-    <t>szr</t>
-  </si>
-  <si>
-    <t>8D35B11AF268DE257C9A97B08BFA9EBC12424307D3B01DB70C7B025050BEACBE</t>
-  </si>
-  <si>
-    <t>szr1</t>
-  </si>
-  <si>
-    <t>szr2</t>
-  </si>
-  <si>
-    <t>719433ACF18C03561A6EEC88E2DC55FB341963061C57C60D1EF7528A8DD693FA</t>
-  </si>
-  <si>
-    <t>2A51E8A420C54DCC6D57A3B739004E9BDFA2481A8ACB183F27E6A541A12B3F34</t>
-  </si>
-  <si>
     <t>gon-flixnet-1</t>
   </si>
   <si>
     <t>elgafar-1</t>
   </si>
   <si>
-    <t>stars1m7cp7grjvz54kkws9y26m0q9rqtd96l2cplqkyr2797qt8nrzursgrksl9</t>
-  </si>
-  <si>
-    <t>282AFFB1D9F9D8D0EBD65C6436A402130D119430F2B82330E628C87A4D4F21EF</t>
-  </si>
-  <si>
-    <t>ibc/7997EBC8FF5602F785722AB16A2F30146FF5F6FCA2BEFA7959980EB72DF66DC5</t>
-  </si>
-  <si>
-    <t>AC12A32C6EB939455BB32ED22CAF584A858B325BAE80F677A15D7B4CFCC758D7</t>
-  </si>
-  <si>
-    <t>5421945DF6D69EBFAD44086093FED32020C9F10E1C65A6A6705327847F33339B</t>
-  </si>
-  <si>
     <t>C16D20B44314B3FBEAC198EDDA69A738937AE90AE5F4E0BD64104F321BF82FB3</t>
   </si>
   <si>
@@ -189,13 +138,199 @@
   </si>
   <si>
     <t>388C83D2189F82AA31DE36A73197E4091CC88DBB44C873B0EBFA67D055342D38</t>
+  </si>
+  <si>
+    <t>FEB45F00A73C4FA24168C4C2E4065E8A6517AF03216FC26A9CE2F56BEB6CA6F8</t>
+  </si>
+  <si>
+    <t>965B04BDEF0CC5E52B2B7B1C5F53D25E16CEF0463A459A8C6505FE5A6FAC543F</t>
+  </si>
+  <si>
+    <t>szryldrm1</t>
+  </si>
+  <si>
+    <t>szryldrm2</t>
+  </si>
+  <si>
+    <t>6B88FED664985C7D692F9DFFEA9888061C484CA3D1FF501CFE5626535EE36CB4</t>
+  </si>
+  <si>
+    <t>5192951227BA5D0995438982D4ED660500859A98383329B1D0C5331544EBB98F</t>
+  </si>
+  <si>
+    <t>ibc/C4174BEC82C9AA253F3F500C98061BD63CFC9BB47DECA1D7E34015DF6B44EE34</t>
+  </si>
+  <si>
+    <t>5551499732F647AA17E8DF46595685835B7DDB20DEFBBFF2195D792EF93B72A8</t>
+  </si>
+  <si>
+    <t>22B61A8338B7F5B0511248BA3769AD5938A6EF98CF83F01894D66D303C54D441</t>
+  </si>
+  <si>
+    <t>stars1ytuv8awr5mcu2velwnptszlsl7agtgvtmt0yvesxvwwyquakuy6sfstnqc</t>
+  </si>
+  <si>
+    <t>6E6D4B2276A0FC770197CD09EF990A67C0D2EE29897C5380F84E92FF0C09A22F</t>
+  </si>
+  <si>
+    <t>ibc/981F1F4DF57C61C4C5BB49C48A48D8C955ABBDCFFC05F56442BC9FF06210C7C1</t>
+  </si>
+  <si>
+    <t>szryldrmA7</t>
+  </si>
+  <si>
+    <t>szryldrmA8</t>
+  </si>
+  <si>
+    <t>szryldrmA9</t>
+  </si>
+  <si>
+    <t>ibc/E85217D8A3C6C26AE2D147BE51C0C42ECC5426A9CBA8D1385C874AE510BAF46B</t>
+  </si>
+  <si>
+    <t>szryldrmA10</t>
+  </si>
+  <si>
+    <t>szryldrmA11</t>
+  </si>
+  <si>
+    <t>szryldrmA12</t>
+  </si>
+  <si>
+    <t>ibc/6D5AF45D31E5071FCCC997F071F2DBCF4B3250CFDC8BE04E4631AFA20A9EE826</t>
+  </si>
+  <si>
+    <t>ibc/75F596C36E480C5C07EF9349085961CDDE8EAD5DCC9BC42A9514569A594EFFAC</t>
+  </si>
+  <si>
+    <t>ibc/2B45259BDAC656B09E879EF6F6E88997D2B5F3669C69E2E6BA8CBF35F517469C</t>
+  </si>
+  <si>
+    <t>ibc/B600CEC60616D9E85B2D1728EF99A1D59961537E7D6097680878A22C52811101</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>56071B76BFBC3883C362788A64902E95DF2F64D7B256DD6A767B89E3BA041B33</t>
+  </si>
+  <si>
+    <t>A13815DB7C84F1973C4FFB1404B341A106322FC465358E3ABF0DBE13409E491F</t>
+  </si>
+  <si>
+    <t>4D4A35508C6BFE13CBD2704949BEB62363AFF3D7179C75110BF4575FBBF218AE</t>
+  </si>
+  <si>
+    <t>F374097271D02D3C8D8A5994CF75F2C1DF33BACA6C14D9A2BDDA929FB0A00A04</t>
+  </si>
+  <si>
+    <t>A44B7181928F340D699AC655EC0C8690F9F270EA29A8DB1FCB044B48B7205986</t>
+  </si>
+  <si>
+    <t>015E6529630ABF33741C188F4C546590A6A9E08023C0ECA41B02816A0E870653</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>EA17B4A0DA613611A2B14EA460D4E36A9327DD6B0E8E1B5D198BBCA95AFAB414</t>
+  </si>
+  <si>
+    <t>D092C2097754848931C6195CD7CCB3AABB74EE6858DC6EB1E5D0445A23CB52E8</t>
+  </si>
+  <si>
+    <t>879D7D1A1BF08D2FB99E19BBA350A2A5955438858258FCDA46CEA348CFF0A4CD</t>
+  </si>
+  <si>
+    <t>F945888BCDA8B8EEB0A748F87052D360FAE15418280B9D6D9E0E1AAC30D3EC24</t>
+  </si>
+  <si>
+    <t>1B28A27F9AC86655F718D4413EA0EA04FE68F524ACED4E6C6A80775109BB52E7</t>
+  </si>
+  <si>
+    <t>C654A2B2765582E0BB931795223D867B8F402FB0AC3BF4E951F00785BD918E61</t>
+  </si>
+  <si>
+    <t>D9A54B32E3A5F805D72CE36D7F85FA544A2179AA255A098BB54D6E58EFF48537</t>
+  </si>
+  <si>
+    <t>FD40ECAAF502CDCA56F03CC09D9236FDB1BDEB24011286C11E7F33C1918A7D54</t>
+  </si>
+  <si>
+    <t>7FF69DC6FD7E7E5FE3DAD6210F6382AB13586F520F00559DBD55CF9B8D393A78</t>
+  </si>
+  <si>
+    <t>95B6DF5B549823D9069BB8CC0C62F6901FEB844A998F5FCD1151AEE4719D793F</t>
+  </si>
+  <si>
+    <t>3456F1F2B6B79AEC359BBD635D6181ACD8F126BFFA7F9B06A7F0E36E8422BECA</t>
+  </si>
+  <si>
+    <t>1340DE0C98DC0BBEFF750761C3062C93582EE07E89564BD8265DF8513EE3247E</t>
+  </si>
+  <si>
+    <t>5D11A11D14F42032DC18C69FDE70B8D6CFBF2582E2B75CA372FC7FD5762EC9F2</t>
+  </si>
+  <si>
+    <t>16759F59A930FE5FF085EBFFFB923ADA514E402FCEBDAD8B0229B6BF739C4869</t>
+  </si>
+  <si>
+    <t>859CA9139580FF0B8AF3FFC2BCB9FB27463C3C0CD32AEF169DCA79558A86ECE4</t>
+  </si>
+  <si>
+    <t>139422EAB86E361FE9F1C83C862BB216894E9AC937D5BC77EDD81BE6AC027DAB</t>
+  </si>
+  <si>
+    <t>CD58C9130CE2E6DCA64891607494EBD23B717615D1C355981B7EDB0650E38BBD</t>
+  </si>
+  <si>
+    <t>9580B4F54D427F56B1A426A20EA84BD49ACFB0E9E8D0A621AF69EADC59DDE7D2</t>
+  </si>
+  <si>
+    <t>986D31B062E41C4A605EDFFD63379D86B8D94928E0D3D588518609C8DDC20E24</t>
+  </si>
+  <si>
+    <t>A411A6EEE4F2CD9EB949C55461F6078AEE6A4751BBE3699B3C88DA7231525F1A</t>
+  </si>
+  <si>
+    <t>FA936B56612DCBEEE849579ED5C7DC2B7EFD9BC1D6B286E82B8436EF5DAE1EBE</t>
+  </si>
+  <si>
+    <t>DBC3C65F7F42D5F167103BB277CF560AAD98434669683562D86F42A535C73695</t>
+  </si>
+  <si>
+    <t>D0BA010F31CC4405766B4927738D7F61EB9234015358869566C0B0F29F51F916</t>
+  </si>
+  <si>
+    <t>1DCD035ECB8F24229B5B43AF74B5A28B1BA3232374E6A9A272619B980CDA0C81</t>
+  </si>
+  <si>
+    <t>A9304E52EE4D0ABE731F6F6CA2EA69E590E6033E9AFBCDAB45ADAFBA4AEF36CF</t>
+  </si>
+  <si>
+    <t>70EC97383DFED187AA7EEFD28A10C70B256969BA2BC007DB19FBFA40C0146D01</t>
+  </si>
+  <si>
+    <t>4441AB516772082E0A52AFC13FC8A94524B1EDB4E7B1821D5EDCD8825B432FCF</t>
+  </si>
+  <si>
+    <t>1611C7E006ED877E7F41537AD7ADC04B2000D1689754AD310F17B8A0F308A200</t>
+  </si>
+  <si>
+    <t>2993ED9C8A879D4DA149EF13989C42CCF736E80633ABB3534D8570F098C8416C</t>
+  </si>
+  <si>
+    <t>AE72430D53F5811A0AC33E86A08EDA4A77B80C08D34BFBB5095E7670FBBBDB50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,9 +340,50 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -259,31 +435,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{40D757D5-B51B-4EE8-8E89-FF7405C88D6A}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{E1F9CB1E-15EA-4FFC-AA33-221E0E4EE4B3}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{B2381EC8-72C3-4B23-B1F7-89C68AF7D23D}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{54CA7D3A-ACC2-4B34-A871-478B2255EA07}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -589,7 +797,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,51 +814,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -666,7 +874,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -676,18 +886,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -702,7 +912,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -712,18 +924,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +950,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -748,18 +962,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -774,7 +988,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -784,18 +1000,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -808,9 +1024,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -828,23 +1046,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -856,9 +1086,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -876,23 +1108,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>81</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,9 +1148,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -924,23 +1170,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -952,9 +1210,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -972,23 +1232,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1000,9 +1272,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1020,23 +1294,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>73</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1048,9 +1334,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1068,23 +1356,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1099,7 +1399,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,15 +1412,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1133,9 +1433,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1153,23 +1455,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>63</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1181,9 +1511,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1200,24 +1532,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1247,12 +1607,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1283,12 +1643,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1319,12 +1679,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1355,12 +1715,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1733,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,12 +1748,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1769,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,35 +1783,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1465,7 +1826,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1491,16 +1852,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1531,10 +1892,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1542,16 +1903,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1582,10 +1943,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1593,16 +1954,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1634,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1645,16 +2006,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1669,7 +2030,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1679,18 +2042,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +2068,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1715,18 +2080,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>